<commit_message>
update month days length
</commit_message>
<xml_diff>
--- a/log.xlsx
+++ b/log.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H436"/>
+  <dimension ref="A1:H444"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -18721,7 +18721,7 @@
       </c>
       <c r="D436" t="inlineStr">
         <is>
-          <t>15:30</t>
+          <t>16:30</t>
         </is>
       </c>
       <c r="E436" t="inlineStr">
@@ -18742,6 +18742,342 @@
       <c r="H436" t="inlineStr">
         <is>
           <t>btn_14</t>
+        </is>
+      </c>
+    </row>
+    <row r="437">
+      <c r="A437" t="inlineStr">
+        <is>
+          <t>LÊ MINH THẮNG</t>
+        </is>
+      </c>
+      <c r="B437" t="inlineStr">
+        <is>
+          <t>223906</t>
+        </is>
+      </c>
+      <c r="C437" t="inlineStr">
+        <is>
+          <t>16:30</t>
+        </is>
+      </c>
+      <c r="D437" t="inlineStr">
+        <is>
+          <t>16:30</t>
+        </is>
+      </c>
+      <c r="E437" t="inlineStr">
+        <is>
+          <t>TEST REQUEST</t>
+        </is>
+      </c>
+      <c r="F437" t="inlineStr">
+        <is>
+          <t>RD</t>
+        </is>
+      </c>
+      <c r="G437" t="inlineStr">
+        <is>
+          <t>2024-05-18</t>
+        </is>
+      </c>
+      <c r="H437" t="inlineStr">
+        <is>
+          <t>btn_12</t>
+        </is>
+      </c>
+    </row>
+    <row r="438">
+      <c r="A438" t="inlineStr">
+        <is>
+          <t>LÊ QUỐC TRUNG</t>
+        </is>
+      </c>
+      <c r="B438" t="inlineStr">
+        <is>
+          <t>224016</t>
+        </is>
+      </c>
+      <c r="C438" t="inlineStr">
+        <is>
+          <t>16:30</t>
+        </is>
+      </c>
+      <c r="D438" t="inlineStr">
+        <is>
+          <t>19:0</t>
+        </is>
+      </c>
+      <c r="E438" t="inlineStr">
+        <is>
+          <t>B/T</t>
+        </is>
+      </c>
+      <c r="F438" t="inlineStr">
+        <is>
+          <t>RD</t>
+        </is>
+      </c>
+      <c r="G438" t="inlineStr">
+        <is>
+          <t>2024-05-18</t>
+        </is>
+      </c>
+      <c r="H438" t="inlineStr">
+        <is>
+          <t>btn_13</t>
+        </is>
+      </c>
+    </row>
+    <row r="439">
+      <c r="A439" t="inlineStr">
+        <is>
+          <t>NGUYỄN HOÀNG VIỆT</t>
+        </is>
+      </c>
+      <c r="B439" t="inlineStr">
+        <is>
+          <t>172759</t>
+        </is>
+      </c>
+      <c r="C439" t="inlineStr">
+        <is>
+          <t>16:30</t>
+        </is>
+      </c>
+      <c r="D439" t="inlineStr">
+        <is>
+          <t>19:30</t>
+        </is>
+      </c>
+      <c r="E439" t="inlineStr">
+        <is>
+          <t>TEST REQUEST</t>
+        </is>
+      </c>
+      <c r="F439" t="inlineStr">
+        <is>
+          <t>RD</t>
+        </is>
+      </c>
+      <c r="G439" t="inlineStr">
+        <is>
+          <t>2024-05-18</t>
+        </is>
+      </c>
+      <c r="H439" t="inlineStr">
+        <is>
+          <t>btn_6</t>
+        </is>
+      </c>
+    </row>
+    <row r="440">
+      <c r="A440" t="inlineStr">
+        <is>
+          <t>TRẦN VĂN LƯU</t>
+        </is>
+      </c>
+      <c r="B440" t="inlineStr">
+        <is>
+          <t>234102</t>
+        </is>
+      </c>
+      <c r="C440" t="inlineStr">
+        <is>
+          <t>16:30</t>
+        </is>
+      </c>
+      <c r="D440" t="inlineStr">
+        <is>
+          <t>19:30</t>
+        </is>
+      </c>
+      <c r="E440" t="inlineStr">
+        <is>
+          <t>TEST REQUEST</t>
+        </is>
+      </c>
+      <c r="F440" t="inlineStr">
+        <is>
+          <t>RD</t>
+        </is>
+      </c>
+      <c r="G440" t="inlineStr">
+        <is>
+          <t>2024-05-18</t>
+        </is>
+      </c>
+      <c r="H440" t="inlineStr">
+        <is>
+          <t>btn_15</t>
+        </is>
+      </c>
+    </row>
+    <row r="441">
+      <c r="A441" t="inlineStr">
+        <is>
+          <t>PHẠM THỊ PHƯƠNG</t>
+        </is>
+      </c>
+      <c r="B441" t="inlineStr">
+        <is>
+          <t>172684</t>
+        </is>
+      </c>
+      <c r="C441" t="inlineStr">
+        <is>
+          <t>16:30</t>
+        </is>
+      </c>
+      <c r="D441" t="inlineStr">
+        <is>
+          <t>19:30</t>
+        </is>
+      </c>
+      <c r="E441" t="inlineStr">
+        <is>
+          <t>TEST REQUEST</t>
+        </is>
+      </c>
+      <c r="F441" t="inlineStr">
+        <is>
+          <t>RD</t>
+        </is>
+      </c>
+      <c r="G441" t="inlineStr">
+        <is>
+          <t>2024-05-18</t>
+        </is>
+      </c>
+      <c r="H441" t="inlineStr">
+        <is>
+          <t>btn_5</t>
+        </is>
+      </c>
+    </row>
+    <row r="442">
+      <c r="A442" t="inlineStr">
+        <is>
+          <t>NGUYỄN QUANG QUÍ</t>
+        </is>
+      </c>
+      <c r="B442" t="inlineStr">
+        <is>
+          <t>203638</t>
+        </is>
+      </c>
+      <c r="C442" t="inlineStr">
+        <is>
+          <t>16:30</t>
+        </is>
+      </c>
+      <c r="D442" t="inlineStr">
+        <is>
+          <t>19:30</t>
+        </is>
+      </c>
+      <c r="E442" t="inlineStr">
+        <is>
+          <t>TEST REQUEST</t>
+        </is>
+      </c>
+      <c r="F442" t="inlineStr">
+        <is>
+          <t>RD</t>
+        </is>
+      </c>
+      <c r="G442" t="inlineStr">
+        <is>
+          <t>2024-05-18</t>
+        </is>
+      </c>
+      <c r="H442" t="inlineStr">
+        <is>
+          <t>btn_10</t>
+        </is>
+      </c>
+    </row>
+    <row r="443">
+      <c r="A443" t="inlineStr">
+        <is>
+          <t>LÊ MINH THẮNG</t>
+        </is>
+      </c>
+      <c r="B443" t="inlineStr">
+        <is>
+          <t>223906</t>
+        </is>
+      </c>
+      <c r="C443" t="inlineStr">
+        <is>
+          <t>7:30</t>
+        </is>
+      </c>
+      <c r="D443" t="inlineStr">
+        <is>
+          <t>16:30</t>
+        </is>
+      </c>
+      <c r="E443" t="inlineStr">
+        <is>
+          <t>TEST REQUEST</t>
+        </is>
+      </c>
+      <c r="F443" t="inlineStr">
+        <is>
+          <t>RD</t>
+        </is>
+      </c>
+      <c r="G443" t="inlineStr">
+        <is>
+          <t>2024-05-19</t>
+        </is>
+      </c>
+      <c r="H443" t="inlineStr">
+        <is>
+          <t>btn_12</t>
+        </is>
+      </c>
+    </row>
+    <row r="444">
+      <c r="A444" t="inlineStr">
+        <is>
+          <t>LÊ HUỲNH ANH KHOA</t>
+        </is>
+      </c>
+      <c r="B444" t="inlineStr">
+        <is>
+          <t>234168</t>
+        </is>
+      </c>
+      <c r="C444" t="inlineStr">
+        <is>
+          <t>7:30</t>
+        </is>
+      </c>
+      <c r="D444" t="inlineStr">
+        <is>
+          <t>16:30</t>
+        </is>
+      </c>
+      <c r="E444" t="inlineStr">
+        <is>
+          <t>B/T</t>
+        </is>
+      </c>
+      <c r="F444" t="inlineStr">
+        <is>
+          <t>RD</t>
+        </is>
+      </c>
+      <c r="G444" t="inlineStr">
+        <is>
+          <t>2024-05-19</t>
+        </is>
+      </c>
+      <c r="H444" t="inlineStr">
+        <is>
+          <t>btn_16</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
update calendar and add setTimeOut for staff submit button
</commit_message>
<xml_diff>
--- a/log.xlsx
+++ b/log.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H444"/>
+  <dimension ref="A1:H453"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -19081,6 +19081,384 @@
         </is>
       </c>
     </row>
+    <row r="445">
+      <c r="A445" t="inlineStr">
+        <is>
+          <t>NGUYỄN TUẤN ANH</t>
+        </is>
+      </c>
+      <c r="B445" t="inlineStr">
+        <is>
+          <t>224057</t>
+        </is>
+      </c>
+      <c r="C445" t="inlineStr">
+        <is>
+          <t>16:30</t>
+        </is>
+      </c>
+      <c r="D445" t="inlineStr">
+        <is>
+          <t>16:30</t>
+        </is>
+      </c>
+      <c r="E445" t="inlineStr">
+        <is>
+          <t>TEST REQUEST</t>
+        </is>
+      </c>
+      <c r="F445" t="inlineStr">
+        <is>
+          <t>RD</t>
+        </is>
+      </c>
+      <c r="G445" t="inlineStr">
+        <is>
+          <t>2024-05-20</t>
+        </is>
+      </c>
+      <c r="H445" t="inlineStr">
+        <is>
+          <t>btn_14</t>
+        </is>
+      </c>
+    </row>
+    <row r="446">
+      <c r="A446" t="inlineStr">
+        <is>
+          <t>PHẠM THỊ PHƯƠNG</t>
+        </is>
+      </c>
+      <c r="B446" t="inlineStr">
+        <is>
+          <t>172684</t>
+        </is>
+      </c>
+      <c r="C446" t="inlineStr">
+        <is>
+          <t>16:30</t>
+        </is>
+      </c>
+      <c r="D446" t="inlineStr">
+        <is>
+          <t>19:30</t>
+        </is>
+      </c>
+      <c r="E446" t="inlineStr">
+        <is>
+          <t>TEST REQUEST</t>
+        </is>
+      </c>
+      <c r="F446" t="inlineStr">
+        <is>
+          <t>RD</t>
+        </is>
+      </c>
+      <c r="G446" t="inlineStr">
+        <is>
+          <t>2024-05-20</t>
+        </is>
+      </c>
+      <c r="H446" t="inlineStr">
+        <is>
+          <t>btn_5</t>
+        </is>
+      </c>
+    </row>
+    <row r="447">
+      <c r="A447" t="inlineStr">
+        <is>
+          <t>TRƯƠNG VĂN MINH</t>
+        </is>
+      </c>
+      <c r="B447" t="inlineStr">
+        <is>
+          <t>203591</t>
+        </is>
+      </c>
+      <c r="C447" t="inlineStr">
+        <is>
+          <t>16:30</t>
+        </is>
+      </c>
+      <c r="D447" t="inlineStr">
+        <is>
+          <t>19:30</t>
+        </is>
+      </c>
+      <c r="E447" t="inlineStr">
+        <is>
+          <t>TEST REQUEST</t>
+        </is>
+      </c>
+      <c r="F447" t="inlineStr">
+        <is>
+          <t>RD</t>
+        </is>
+      </c>
+      <c r="G447" t="inlineStr">
+        <is>
+          <t>2024-05-20</t>
+        </is>
+      </c>
+      <c r="H447" t="inlineStr">
+        <is>
+          <t>btn_9</t>
+        </is>
+      </c>
+    </row>
+    <row r="448">
+      <c r="A448" t="inlineStr">
+        <is>
+          <t>LÊ MINH THẮNG</t>
+        </is>
+      </c>
+      <c r="B448" t="inlineStr">
+        <is>
+          <t>223906</t>
+        </is>
+      </c>
+      <c r="C448" t="inlineStr">
+        <is>
+          <t>16:30</t>
+        </is>
+      </c>
+      <c r="D448" t="inlineStr">
+        <is>
+          <t>19:30</t>
+        </is>
+      </c>
+      <c r="E448" t="inlineStr">
+        <is>
+          <t>TEST REQUEST</t>
+        </is>
+      </c>
+      <c r="F448" t="inlineStr">
+        <is>
+          <t>RD</t>
+        </is>
+      </c>
+      <c r="G448" t="inlineStr">
+        <is>
+          <t>2024-05-20</t>
+        </is>
+      </c>
+      <c r="H448" t="inlineStr">
+        <is>
+          <t>btn_12</t>
+        </is>
+      </c>
+    </row>
+    <row r="449">
+      <c r="A449" t="inlineStr">
+        <is>
+          <t>NGUYỄN HOÀNG VIỆT</t>
+        </is>
+      </c>
+      <c r="B449" t="inlineStr">
+        <is>
+          <t>172759</t>
+        </is>
+      </c>
+      <c r="C449" t="inlineStr">
+        <is>
+          <t>16:30</t>
+        </is>
+      </c>
+      <c r="D449" t="inlineStr">
+        <is>
+          <t>19:30</t>
+        </is>
+      </c>
+      <c r="E449" t="inlineStr">
+        <is>
+          <t>TEST REQUEST</t>
+        </is>
+      </c>
+      <c r="F449" t="inlineStr">
+        <is>
+          <t>RD</t>
+        </is>
+      </c>
+      <c r="G449" t="inlineStr">
+        <is>
+          <t>2024-05-20</t>
+        </is>
+      </c>
+      <c r="H449" t="inlineStr">
+        <is>
+          <t>btn_6</t>
+        </is>
+      </c>
+    </row>
+    <row r="450">
+      <c r="A450" t="inlineStr">
+        <is>
+          <t>TRẦN VĂN LƯU</t>
+        </is>
+      </c>
+      <c r="B450" t="inlineStr">
+        <is>
+          <t>234102</t>
+        </is>
+      </c>
+      <c r="C450" t="inlineStr">
+        <is>
+          <t>16:30</t>
+        </is>
+      </c>
+      <c r="D450" t="inlineStr">
+        <is>
+          <t>19:30</t>
+        </is>
+      </c>
+      <c r="E450" t="inlineStr">
+        <is>
+          <t>TEST REQUEST</t>
+        </is>
+      </c>
+      <c r="F450" t="inlineStr">
+        <is>
+          <t>RD</t>
+        </is>
+      </c>
+      <c r="G450" t="inlineStr">
+        <is>
+          <t>2024-05-20</t>
+        </is>
+      </c>
+      <c r="H450" t="inlineStr">
+        <is>
+          <t>btn_15</t>
+        </is>
+      </c>
+    </row>
+    <row r="451">
+      <c r="A451" t="inlineStr">
+        <is>
+          <t>LÊ HUỲNH ANH KHOA</t>
+        </is>
+      </c>
+      <c r="B451" t="inlineStr">
+        <is>
+          <t>234168</t>
+        </is>
+      </c>
+      <c r="C451" t="inlineStr">
+        <is>
+          <t>16:30</t>
+        </is>
+      </c>
+      <c r="D451" t="inlineStr">
+        <is>
+          <t>19:30</t>
+        </is>
+      </c>
+      <c r="E451" t="inlineStr">
+        <is>
+          <t>B/T</t>
+        </is>
+      </c>
+      <c r="F451" t="inlineStr">
+        <is>
+          <t>RD</t>
+        </is>
+      </c>
+      <c r="G451" t="inlineStr">
+        <is>
+          <t>2024-05-20</t>
+        </is>
+      </c>
+      <c r="H451" t="inlineStr">
+        <is>
+          <t>btn_16</t>
+        </is>
+      </c>
+    </row>
+    <row r="452">
+      <c r="A452" t="inlineStr">
+        <is>
+          <t>NGUYỄN QUANG QUÍ</t>
+        </is>
+      </c>
+      <c r="B452" t="inlineStr">
+        <is>
+          <t>203638</t>
+        </is>
+      </c>
+      <c r="C452" t="inlineStr">
+        <is>
+          <t>16:30</t>
+        </is>
+      </c>
+      <c r="D452" t="inlineStr">
+        <is>
+          <t>19:30</t>
+        </is>
+      </c>
+      <c r="E452" t="inlineStr">
+        <is>
+          <t>TEST REQUEST</t>
+        </is>
+      </c>
+      <c r="F452" t="inlineStr">
+        <is>
+          <t>RD</t>
+        </is>
+      </c>
+      <c r="G452" t="inlineStr">
+        <is>
+          <t>2024-05-20</t>
+        </is>
+      </c>
+      <c r="H452" t="inlineStr">
+        <is>
+          <t>btn_10</t>
+        </is>
+      </c>
+    </row>
+    <row r="453">
+      <c r="A453" t="inlineStr">
+        <is>
+          <t>NGUYỄN TUẤN ANH</t>
+        </is>
+      </c>
+      <c r="B453" t="inlineStr">
+        <is>
+          <t>224057</t>
+        </is>
+      </c>
+      <c r="C453" t="inlineStr">
+        <is>
+          <t>16:30</t>
+        </is>
+      </c>
+      <c r="D453" t="inlineStr">
+        <is>
+          <t>14:30</t>
+        </is>
+      </c>
+      <c r="E453" t="inlineStr">
+        <is>
+          <t>TEST REQUEST</t>
+        </is>
+      </c>
+      <c r="F453" t="inlineStr">
+        <is>
+          <t>RD</t>
+        </is>
+      </c>
+      <c r="G453" t="inlineStr">
+        <is>
+          <t>2024-05-21</t>
+        </is>
+      </c>
+      <c r="H453" t="inlineStr">
+        <is>
+          <t>btn_14</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>